<commit_message>
update PATHS in nodegoat scripts and rename nodegoat scripts to process_data
</commit_message>
<xml_diff>
--- a/data/raw/Image.xlsx
+++ b/data/raw/Image.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1D5D19-DFCF-884A-ADB0-7D0895E2D36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C56066-00E6-2B4B-9B36-BBFDD70D94B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="620" windowWidth="66540" windowHeight="31380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="620" windowWidth="76380" windowHeight="31380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="512">
   <si>
     <t>ID</t>
   </si>
@@ -1566,6 +1566,15 @@
   </si>
   <si>
     <t>Executioners and crowd collecting round Cheshire Cat</t>
+  </si>
+  <si>
+    <t>Multimedia Folder</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>image_alternative</t>
   </si>
 </sst>
 </file>
@@ -1658,7 +1667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1674,6 +1683,7 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1870,10 +1880,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N104"/>
+  <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F1:F1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N93" sqref="N93:N104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1894,7 +1904,7 @@
     <col min="14" max="14" width="33" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1937,8 +1947,11 @@
       <c r="N1" s="8" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="13" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>260</v>
       </c>
@@ -1979,8 +1992,11 @@
       <c r="N2" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>368</v>
       </c>
@@ -2021,8 +2037,11 @@
       <c r="N3" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>55</v>
       </c>
@@ -2063,8 +2082,11 @@
       <c r="N4" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
@@ -2105,8 +2127,11 @@
       <c r="N5" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
@@ -2147,8 +2172,11 @@
       <c r="N6" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>372</v>
       </c>
@@ -2189,8 +2217,11 @@
       <c r="N7" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>131</v>
       </c>
@@ -2231,8 +2262,11 @@
       <c r="N8" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2273,8 +2307,11 @@
       <c r="N9" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O9" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>280</v>
       </c>
@@ -2315,8 +2352,11 @@
       <c r="N10" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O10" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -2357,8 +2397,11 @@
       <c r="N11" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O11" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -2399,8 +2442,11 @@
       <c r="N12" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O12" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>143</v>
       </c>
@@ -2441,8 +2487,11 @@
       <c r="N13" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O13" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>147</v>
       </c>
@@ -2483,8 +2532,11 @@
       <c r="N14" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O14" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>316</v>
       </c>
@@ -2525,8 +2577,11 @@
       <c r="N15" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O15" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>167</v>
       </c>
@@ -2567,8 +2622,11 @@
       <c r="N16" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O16" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>204</v>
       </c>
@@ -2609,8 +2667,11 @@
       <c r="N17" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O17" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>208</v>
       </c>
@@ -2651,8 +2712,11 @@
       <c r="N18" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O18" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>200</v>
       </c>
@@ -2693,8 +2757,11 @@
       <c r="N19" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O19" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>196</v>
       </c>
@@ -2735,8 +2802,11 @@
       <c r="N20" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O20" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>212</v>
       </c>
@@ -2777,8 +2847,11 @@
       <c r="N21" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O21" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>189</v>
       </c>
@@ -2819,8 +2892,11 @@
       <c r="N22" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O22" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>79</v>
       </c>
@@ -2861,8 +2937,11 @@
       <c r="N23" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O23" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>174</v>
       </c>
@@ -2903,8 +2982,11 @@
       <c r="N24" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>171</v>
       </c>
@@ -2945,8 +3027,11 @@
       <c r="N25" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O25" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>127</v>
       </c>
@@ -2987,8 +3072,11 @@
       <c r="N26" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O26" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>240</v>
       </c>
@@ -3029,8 +3117,11 @@
       <c r="N27" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O27" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>185</v>
       </c>
@@ -3071,8 +3162,11 @@
       <c r="N28" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O28" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>159</v>
       </c>
@@ -3113,8 +3207,11 @@
       <c r="N29" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O29" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>288</v>
       </c>
@@ -3155,8 +3252,11 @@
       <c r="N30" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O30" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>71</v>
       </c>
@@ -3197,8 +3297,11 @@
       <c r="N31" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O31" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>193</v>
       </c>
@@ -3239,8 +3342,11 @@
       <c r="N32" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O32" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>19</v>
       </c>
@@ -3281,8 +3387,11 @@
       <c r="N33" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O33" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>216</v>
       </c>
@@ -3323,8 +3432,11 @@
       <c r="N34" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O34" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>276</v>
       </c>
@@ -3365,8 +3477,11 @@
       <c r="N35" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O35" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>272</v>
       </c>
@@ -3407,8 +3522,11 @@
       <c r="N36" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O36" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>268</v>
       </c>
@@ -3449,8 +3567,11 @@
       <c r="N37" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O37" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>364</v>
       </c>
@@ -3491,8 +3612,11 @@
       <c r="N38" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O38" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>236</v>
       </c>
@@ -3533,8 +3657,11 @@
       <c r="N39" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O39" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>232</v>
       </c>
@@ -3575,8 +3702,11 @@
       <c r="N40" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O40" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>135</v>
       </c>
@@ -3617,8 +3747,11 @@
       <c r="N41" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O41" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>264</v>
       </c>
@@ -3659,8 +3792,11 @@
       <c r="N42" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O42" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>163</v>
       </c>
@@ -3701,8 +3837,11 @@
       <c r="N43" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O43" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>356</v>
       </c>
@@ -3743,8 +3882,11 @@
       <c r="N44" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O44" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>151</v>
       </c>
@@ -3785,8 +3927,11 @@
       <c r="N45" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O45" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>139</v>
       </c>
@@ -3827,8 +3972,11 @@
       <c r="N46" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O46" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>59</v>
       </c>
@@ -3869,8 +4017,11 @@
       <c r="N47" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O47" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
@@ -3911,8 +4062,11 @@
       <c r="N48" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O48" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>181</v>
       </c>
@@ -3953,8 +4107,11 @@
       <c r="N49" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O49" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>99</v>
       </c>
@@ -3995,8 +4152,11 @@
       <c r="N50" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O50" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>320</v>
       </c>
@@ -4037,8 +4197,11 @@
       <c r="N51" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O51" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>256</v>
       </c>
@@ -4079,8 +4242,11 @@
       <c r="N52" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O52" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>324</v>
       </c>
@@ -4121,8 +4287,11 @@
       <c r="N53" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O53" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>31</v>
       </c>
@@ -4163,8 +4332,11 @@
       <c r="N54" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O54" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>177</v>
       </c>
@@ -4203,8 +4375,11 @@
       <c r="N55" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O55" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -4245,8 +4420,11 @@
       <c r="N56" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O56" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>123</v>
       </c>
@@ -4287,8 +4465,11 @@
       <c r="N57" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O57" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>308</v>
       </c>
@@ -4327,8 +4508,11 @@
       <c r="N58" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O58" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>312</v>
       </c>
@@ -4367,8 +4551,11 @@
       <c r="N59" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O59" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>155</v>
       </c>
@@ -4407,8 +4594,11 @@
       <c r="N60" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O60" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>43</v>
       </c>
@@ -4449,8 +4639,11 @@
       <c r="N61" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O61" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>39</v>
       </c>
@@ -4491,8 +4684,11 @@
       <c r="N62" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O62" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>344</v>
       </c>
@@ -4533,8 +4729,11 @@
       <c r="N63" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O63" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>340</v>
       </c>
@@ -4575,8 +4774,11 @@
       <c r="N64" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O64" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>336</v>
       </c>
@@ -4617,8 +4819,11 @@
       <c r="N65" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O65" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>292</v>
       </c>
@@ -4659,8 +4864,11 @@
       <c r="N66" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O66" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>332</v>
       </c>
@@ -4701,8 +4909,11 @@
       <c r="N67" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O67" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>328</v>
       </c>
@@ -4743,8 +4954,11 @@
       <c r="N68" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O68" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>14</v>
       </c>
@@ -4785,8 +4999,11 @@
       <c r="N69" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O69" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>228</v>
       </c>
@@ -4827,8 +5044,11 @@
       <c r="N70" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O70" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>83</v>
       </c>
@@ -4869,8 +5089,11 @@
       <c r="N71" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O71" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>111</v>
       </c>
@@ -4911,8 +5134,11 @@
       <c r="N72" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O72" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>244</v>
       </c>
@@ -4953,8 +5179,11 @@
       <c r="N73" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O73" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>252</v>
       </c>
@@ -4993,8 +5222,11 @@
       <c r="N74" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O74" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>248</v>
       </c>
@@ -5035,8 +5267,11 @@
       <c r="N75" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O75" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>348</v>
       </c>
@@ -5075,8 +5310,11 @@
       <c r="N76" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O76" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>220</v>
       </c>
@@ -5117,8 +5355,11 @@
       <c r="N77" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O77" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>224</v>
       </c>
@@ -5159,8 +5400,11 @@
       <c r="N78" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O78" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>67</v>
       </c>
@@ -5201,8 +5445,11 @@
       <c r="N79" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O79" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>107</v>
       </c>
@@ -5243,8 +5490,11 @@
       <c r="N80" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O80" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>296</v>
       </c>
@@ -5285,8 +5535,11 @@
       <c r="N81" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O81" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>352</v>
       </c>
@@ -5327,8 +5580,11 @@
       <c r="N82" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O82" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>51</v>
       </c>
@@ -5369,8 +5625,11 @@
       <c r="N83" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O83" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>360</v>
       </c>
@@ -5411,8 +5670,11 @@
       <c r="N84" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O84" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>87</v>
       </c>
@@ -5453,8 +5715,11 @@
       <c r="N85" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O85" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>300</v>
       </c>
@@ -5495,8 +5760,11 @@
       <c r="N86" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O86" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>304</v>
       </c>
@@ -5537,8 +5805,11 @@
       <c r="N87" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O87" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>23</v>
       </c>
@@ -5579,8 +5850,11 @@
       <c r="N88" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O88" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>284</v>
       </c>
@@ -5619,8 +5893,11 @@
       <c r="N89" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O89" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>103</v>
       </c>
@@ -5661,8 +5938,11 @@
       <c r="N90" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O90" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>119</v>
       </c>
@@ -5703,8 +5983,11 @@
       <c r="N91" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O91" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>115</v>
       </c>
@@ -5745,8 +6028,11 @@
       <c r="N92" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O92" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>91</v>
       </c>
@@ -5787,8 +6073,11 @@
       <c r="N93" s="8" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93" s="13" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>477</v>
       </c>
@@ -5822,8 +6111,14 @@
       <c r="L94" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N94" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O94" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>478</v>
       </c>
@@ -5857,8 +6152,14 @@
       <c r="L95" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N95" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O95" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>479</v>
       </c>
@@ -5892,8 +6193,14 @@
       <c r="L96" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N96" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O96" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>480</v>
       </c>
@@ -5927,8 +6234,14 @@
       <c r="L97" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N97" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O97" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>481</v>
       </c>
@@ -5962,8 +6275,14 @@
       <c r="L98" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N98" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O98" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>482</v>
       </c>
@@ -5997,8 +6316,14 @@
       <c r="L99" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N99" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O99" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>483</v>
       </c>
@@ -6032,8 +6357,14 @@
       <c r="L100" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N100" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O100" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>484</v>
       </c>
@@ -6067,8 +6398,14 @@
       <c r="L101" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N101" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O101" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>485</v>
       </c>
@@ -6102,8 +6439,14 @@
       <c r="L102" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N102" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O102" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>486</v>
       </c>
@@ -6137,8 +6480,14 @@
       <c r="L103" s="8" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N103" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O103" s="13" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>487</v>
       </c>
@@ -6171,6 +6520,12 @@
       </c>
       <c r="L104" s="8" t="s">
         <v>499</v>
+      </c>
+      <c r="N104" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="O104" s="13" t="s">
+        <v>511</v>
       </c>
     </row>
   </sheetData>

</xml_diff>